<commit_message>
add bom and gerber
</commit_message>
<xml_diff>
--- a/PCB/prototypeBoard/BOM.xlsx
+++ b/PCB/prototypeBoard/BOM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sundeqing/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sundeqing/Documents/Github/brooklynresearchprojects/inductionLoopProj/PCB/prototypeBoard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{88C1B16E-830C-724E-B93E-F6E88DA094A9}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C351855-D339-8543-836C-15B4CBDA66DA}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5580" yWindow="3560" windowWidth="27640" windowHeight="16940" xr2:uid="{F461FE04-E38E-F541-B05D-64AD0E06E945}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="nrf52withamp" localSheetId="0">Sheet2!$A$1:$M$39</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{9168280E-4CB6-A84B-A802-1C43A7856792}" name="nrf52withamp" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="nrf52withamp" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/sundeqing/Documents/Github/brooklynresearchprojects/inductionLoopProj/PCB/prototypeBoard/nrf52withamp.csv" tab="0" semicolon="1">
       <textFields count="13">
         <textField/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="185">
   <si>
     <t>Qty</t>
   </si>
@@ -604,6 +604,9 @@
   </si>
   <si>
     <t>C30, C37</t>
+  </si>
+  <si>
+    <t>10 sets count</t>
   </si>
 </sst>
 </file>
@@ -659,7 +662,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="nrf52withamp" connectionId="1" xr16:uid="{8D2D3421-9DFC-6D4E-A70E-57CA6E67ACB3}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="nrf52withamp" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -959,10 +962,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{569D4191-8F75-734F-B760-9B8A28FB7CEC}">
-  <dimension ref="A1:L39"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -980,7 +983,7 @@
     <col min="12" max="12" width="7.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1017,8 +1020,11 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>4</v>
       </c>
@@ -1040,8 +1046,12 @@
       <c r="H2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2">
+        <f t="shared" ref="M2:M39" si="0">A2*10</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>6</v>
       </c>
@@ -1066,8 +1076,12 @@
       <c r="K3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M3">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>4</v>
       </c>
@@ -1092,8 +1106,12 @@
       <c r="K4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M4">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1118,8 +1136,12 @@
       <c r="K5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>11</v>
       </c>
@@ -1144,8 +1166,12 @@
       <c r="K6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1167,8 +1193,12 @@
       <c r="H7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1190,8 +1220,12 @@
       <c r="H8" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1216,8 +1250,12 @@
       <c r="K9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1242,8 +1280,12 @@
       <c r="K10" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M10">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>5</v>
       </c>
@@ -1268,8 +1310,12 @@
       <c r="K11" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M11">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1294,8 +1340,12 @@
       <c r="K12" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1320,8 +1370,12 @@
       <c r="K13" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M13">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>4</v>
       </c>
@@ -1343,8 +1397,12 @@
       <c r="H14" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M14">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1369,8 +1427,12 @@
       <c r="K15" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M15">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1395,8 +1457,12 @@
       <c r="K16" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M16">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1421,8 +1487,12 @@
       <c r="K17" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M17">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1444,8 +1514,12 @@
       <c r="H18" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M18">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1467,8 +1541,12 @@
       <c r="H19" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M19">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>4</v>
       </c>
@@ -1493,8 +1571,12 @@
       <c r="K20" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M20">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1519,8 +1601,12 @@
       <c r="K21" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M21">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2</v>
       </c>
@@ -1542,8 +1628,12 @@
       <c r="H22" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M22">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1565,8 +1655,12 @@
       <c r="G23" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M23">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1588,8 +1682,12 @@
       <c r="H24" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M24">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1</v>
       </c>
@@ -1611,8 +1709,12 @@
       <c r="G25" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M25">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1634,8 +1736,12 @@
       <c r="H26" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M26">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1</v>
       </c>
@@ -1654,8 +1760,12 @@
       <c r="F27" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M27">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>4</v>
       </c>
@@ -1677,8 +1787,12 @@
       <c r="H28" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M28">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1700,8 +1814,12 @@
       <c r="G29" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M29">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1729,8 +1847,12 @@
       <c r="L30" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M30">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1</v>
       </c>
@@ -1749,8 +1871,12 @@
       <c r="H31" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M31">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1</v>
       </c>
@@ -1772,8 +1898,12 @@
       <c r="H32" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="M32">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1</v>
       </c>
@@ -1795,8 +1925,12 @@
       <c r="G33" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="M33">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1</v>
       </c>
@@ -1818,8 +1952,12 @@
       <c r="H34" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="M34">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>2</v>
       </c>
@@ -1841,8 +1979,12 @@
       <c r="H35" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="M35">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1</v>
       </c>
@@ -1864,8 +2006,12 @@
       <c r="H36" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="M36">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1</v>
       </c>
@@ -1887,8 +2033,12 @@
       <c r="G37" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="M37">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1</v>
       </c>
@@ -1913,8 +2063,12 @@
       <c r="I38" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="M38">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>2</v>
       </c>
@@ -1932,6 +2086,10 @@
       </c>
       <c r="F39" t="s">
         <v>67</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>